<commit_message>
GPLIM-4825 Handle tubes w UMI and add spacer to output
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/UMIReagents.xlsx
+++ b/mercury/src/test/resources/testdata/UMIReagents.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27022"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="100" windowWidth="12520" windowHeight="16820"/>
+    <workbookView xWindow="0" yWindow="100" windowWidth="22300" windowHeight="16820"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,16 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t>plate barcode</t>
-  </si>
-  <si>
-    <t>length</t>
-  </si>
-  <si>
-    <t>location</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
   <si>
     <t>Inline First Read</t>
   </si>
@@ -39,6 +30,33 @@
   </si>
   <si>
     <t>Before Second Index Read</t>
+  </si>
+  <si>
+    <t>MatrixTube075</t>
+  </si>
+  <si>
+    <t>Spacer Length</t>
+  </si>
+  <si>
+    <t>Eppendorf96</t>
+  </si>
+  <si>
+    <t>UMI Length</t>
+  </si>
+  <si>
+    <t>Vessel Type</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Barcode</t>
+  </si>
+  <si>
+    <t>Before First Read</t>
+  </si>
+  <si>
+    <t>Before Second Read</t>
   </si>
 </sst>
 </file>
@@ -108,8 +126,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -129,19 +169,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -434,71 +496,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>34567</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2">
-        <v>12345</v>
-      </c>
-      <c r="B2">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>66789</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>77891</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3">
-        <v>34567</v>
-      </c>
-      <c r="B3" s="1">
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+      <c r="B6">
+        <v>87654</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4">
-        <v>66789</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5">
-        <v>77891</v>
-      </c>
-      <c r="B5">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>87654</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GPLIM-4825 ignore the pipeline for now and clean up DB model
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/UMIReagents.xlsx
+++ b/mercury/src/test/resources/testdata/UMIReagents.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Inline First Read</t>
   </si>
@@ -126,8 +126,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -169,7 +173,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -187,6 +191,8 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -204,6 +210,8 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -628,6 +636,23 @@
       </c>
       <c r="E7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>77891</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GPLIM-4825 resolve conflict when committing e1b9841d44f
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/UMIReagents.xlsx
+++ b/mercury/src/test/resources/testdata/UMIReagents.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Inline First Read</t>
   </si>
@@ -126,8 +126,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -169,7 +173,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -187,6 +191,8 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -204,6 +210,8 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -628,6 +636,23 @@
       </c>
       <c r="E7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>77891</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GPLIM-5351 fingerprinting metrics and ROX
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/UMIReagents.xlsx
+++ b/mercury/src/test/resources/testdata/UMIReagents.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27022"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="100" windowWidth="22300" windowHeight="16820"/>
@@ -21,26 +21,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Inline First Read</t>
   </si>
   <si>
-    <t>Inline Second Read</t>
-  </si>
-  <si>
-    <t>Before Second Index Read</t>
-  </si>
-  <si>
     <t>MatrixTube075</t>
   </si>
   <si>
     <t>Spacer Length</t>
   </si>
   <si>
-    <t>Eppendorf96</t>
-  </si>
-  <si>
     <t>UMI Length</t>
   </si>
   <si>
@@ -53,10 +44,10 @@
     <t>Barcode</t>
   </si>
   <si>
-    <t>Before First Read</t>
-  </si>
-  <si>
     <t>Before Second Read</t>
+  </si>
+  <si>
+    <t>UMIADAPTERU</t>
   </si>
 </sst>
 </file>
@@ -70,12 +61,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF222222"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -108,6 +93,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -128,50 +118,50 @@
   </borders>
   <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -504,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -519,140 +509,55 @@
     <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="3" customFormat="1">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="2" t="s">
+    <row r="1" spans="1:5" s="2" customFormat="1">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>12345</v>
-      </c>
       <c r="C2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>34567</v>
-      </c>
-      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3" s="1">
-        <v>1</v>
+      <c r="D3">
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>66789</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>77891</v>
-      </c>
-      <c r="C5">
-        <v>9</v>
-      </c>
-      <c r="D5">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>87654</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>87654</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>77891</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GPLIM-6871 revert UMIReagents.xlsx to working version; handle absence of fingerprint metrics
</commit_message>
<xml_diff>
--- a/mercury/src/test/resources/testdata/UMIReagents.xlsx
+++ b/mercury/src/test/resources/testdata/UMIReagents.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="28705"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="27022"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="100" windowWidth="22300" windowHeight="16820"/>
@@ -21,17 +21,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
   <si>
     <t>Inline First Read</t>
   </si>
   <si>
+    <t>Inline Second Read</t>
+  </si>
+  <si>
+    <t>Before Second Index Read</t>
+  </si>
+  <si>
     <t>MatrixTube075</t>
   </si>
   <si>
     <t>Spacer Length</t>
   </si>
   <si>
+    <t>Eppendorf96</t>
+  </si>
+  <si>
     <t>UMI Length</t>
   </si>
   <si>
@@ -44,10 +53,10 @@
     <t>Barcode</t>
   </si>
   <si>
+    <t>Before First Read</t>
+  </si>
+  <si>
     <t>Before Second Read</t>
-  </si>
-  <si>
-    <t>UMIADAPTERU</t>
   </si>
 </sst>
 </file>
@@ -61,6 +70,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -93,11 +108,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Helvetica Neue"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -118,50 +128,50 @@
   </borders>
   <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -494,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -509,55 +519,140 @@
     <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:5" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2">
+        <v>12345</v>
+      </c>
+      <c r="C2">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D2">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>3</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>34567</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>66789</v>
+      </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>77891</v>
+      </c>
+      <c r="C5">
+        <v>9</v>
+      </c>
+      <c r="D5">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="E5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>87654</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>87654</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>77891</v>
+      </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>